<commit_message>
add KAMA indicator (#205)
* add KAMA indicator
</commit_message>
<xml_diff>
--- a/indicators/Kama/Kama.Calc.xlsx
+++ b/indicators/Kama/Kama.Calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F40E626-E528-49E1-8306-7A19EC42BC31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88EF15FA-9064-4C82-A0F1-87FB6C9C3953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,9 +93,9 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -612,30 +612,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="174" fontId="1" fillId="32" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="32" borderId="0" xfId="43" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,7 +703,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -727,7 +727,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="167" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -747,7 +747,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="172" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -767,7 +767,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="172" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:U503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>